<commit_message>
feat: add more import student  tabs
</commit_message>
<xml_diff>
--- a/public/template/student.xlsx
+++ b/public/template/student.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\Senior\inu-garden\public\template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\porst\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF438591-2447-4679-BF38-E02DB66B69FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{87B54719-AE59-424C-BD1B-0E622E173F20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{414DB501-AAAC-40B4-8AF8-BA5EEFADAE51}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{E06D3729-24B1-455F-A1D9-8A924A109395}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,46 +36,68 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+  <si>
+    <t>_kmuttId</t>
+  </si>
+  <si>
+    <t>firstName</t>
+  </si>
   <si>
     <t>lastName</t>
   </si>
   <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>programmeName</t>
+  </si>
+  <si>
+    <t>departmentName</t>
+  </si>
+  <si>
+    <t>GPAX</t>
+  </si>
+  <si>
+    <t>mathGPA</t>
+  </si>
+  <si>
+    <t>engGPA</t>
+  </si>
+  <si>
+    <t>sciGPA</t>
+  </si>
+  <si>
+    <t>school</t>
+  </si>
+  <si>
+    <t>city</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
     <t>admission</t>
   </si>
   <si>
-    <t>email</t>
-  </si>
-  <si>
-    <t>gpax</t>
-  </si>
-  <si>
-    <t>gpaMath</t>
-  </si>
-  <si>
-    <t>gpaEng</t>
-  </si>
-  <si>
-    <t>gpaSci</t>
-  </si>
-  <si>
-    <t>school</t>
-  </si>
-  <si>
-    <t>city</t>
-  </si>
-  <si>
-    <t>_firstName</t>
+    <t>remark</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+      <charset val="222"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Tahoma"/>
       <family val="2"/>
       <charset val="222"/>
@@ -106,7 +128,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="ปกติ" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -122,26 +144,31 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C340D028-A6BC-476B-89BB-98C9B05D0AAC}" name="Table1" displayName="Table1" ref="A1:J2" totalsRowShown="0">
-  <autoFilter ref="A1:J2" xr:uid="{C340D028-A6BC-476B-89BB-98C9B05D0AAC}"/>
-  <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{72F824D6-DDD5-463E-BCE1-41046255AC1F}" name="_firstName"/>
-    <tableColumn id="2" xr3:uid="{C43F0E8F-78A4-4D9B-BA66-A5FBA2AA16ED}" name="lastName"/>
-    <tableColumn id="3" xr3:uid="{1DD12775-4506-406F-9B15-3585C9646C65}" name="admission"/>
-    <tableColumn id="4" xr3:uid="{D9FA8383-3A33-4209-B987-7BFBBA7BA20C}" name="email"/>
-    <tableColumn id="5" xr3:uid="{225FD6D6-3DA8-48C2-9A41-ACC4D20F9FD8}" name="gpax"/>
-    <tableColumn id="6" xr3:uid="{5E124DC4-DE3A-43D9-AD21-D4C9C0D5B9D9}" name="gpaMath"/>
-    <tableColumn id="7" xr3:uid="{2865CF43-8928-47DD-B943-722B325A9E06}" name="gpaEng"/>
-    <tableColumn id="8" xr3:uid="{40E83756-3117-4881-8A24-651F71EC5ADB}" name="gpaSci"/>
-    <tableColumn id="9" xr3:uid="{D7BEBB19-61CB-4580-937B-1AC01AFCF281}" name="school"/>
-    <tableColumn id="10" xr3:uid="{7C23B252-10CA-49DA-95F0-8C7FB0ED914F}" name="city"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E4D57D41-4658-4F9A-A1CC-198C4DD53427}" name="Table1" displayName="Table1" ref="A1:O5" totalsRowShown="0">
+  <autoFilter ref="A1:O5" xr:uid="{E4D57D41-4658-4F9A-A1CC-198C4DD53427}"/>
+  <tableColumns count="15">
+    <tableColumn id="1" xr3:uid="{028004D7-3A69-4523-87A1-68CF6E869053}" name="_kmuttId"/>
+    <tableColumn id="2" xr3:uid="{EAA05EBA-9759-409B-9C20-C3B8155A346B}" name="firstName"/>
+    <tableColumn id="3" xr3:uid="{35C1193D-E866-46B3-9F5C-4BCA1940B994}" name="lastName"/>
+    <tableColumn id="4" xr3:uid="{4B6C0B4F-8312-4AC7-956F-637EB90D4420}" name="email"/>
+    <tableColumn id="5" xr3:uid="{D1A77C9F-4121-4044-9777-3CC8A831A8BE}" name="programmeName"/>
+    <tableColumn id="6" xr3:uid="{97714BCE-70AE-4AEC-AEDC-5CC276E76F3E}" name="departmentName"/>
+    <tableColumn id="7" xr3:uid="{BAACBD44-E6C7-4B02-873F-D278FE1B454C}" name="GPAX"/>
+    <tableColumn id="8" xr3:uid="{3044A7CD-7693-4F9C-A858-C99DD4D0F8F4}" name="mathGPA"/>
+    <tableColumn id="9" xr3:uid="{4F07DC25-F1DD-4ACE-A2BA-4C88CF734766}" name="engGPA"/>
+    <tableColumn id="10" xr3:uid="{256BE1A1-5DFE-4F33-BD1C-D9D92A006AB6}" name="sciGPA"/>
+    <tableColumn id="11" xr3:uid="{BBAAB4EF-C5D7-43DA-AE91-086326E6056A}" name="school"/>
+    <tableColumn id="12" xr3:uid="{03B42524-90D7-4706-ADCB-658D812F8DE0}" name="city"/>
+    <tableColumn id="13" xr3:uid="{77018516-9837-41D2-9ADE-50F09F5B305F}" name="year"/>
+    <tableColumn id="14" xr3:uid="{C1AFFF39-B812-451E-A2EF-4FEAB02A3BBD}" name="admission"/>
+    <tableColumn id="15" xr3:uid="{98054E79-D568-4763-9C23-BB4BCB2BB717}" name="remark"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="ธีมของ Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -151,39 +178,39 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="44546A"/>
+        <a:srgbClr val="0E2841"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
+        <a:srgbClr val="E8E8E8"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="156082"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="ED7D31"/>
+        <a:srgbClr val="E97132"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
+        <a:srgbClr val="196B24"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="FFC000"/>
+        <a:srgbClr val="0F9ED5"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="A02B93"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="70AD47"/>
+        <a:srgbClr val="4EA72E"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0563C1"/>
+        <a:srgbClr val="467886"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="954F72"/>
+        <a:srgbClr val="96607D"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Aptos Display" panose="02110004020202020204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -235,7 +262,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Aptos Narrow" panose="02110004020202020204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -346,13 +373,6 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
         <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
@@ -361,6 +381,13 @@
           <a:miter lim="800000"/>
         </a:ln>
         <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -425,63 +452,99 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults/>
+  <a:objectDefaults>
+    <a:lnDef>
+      <a:spPr/>
+      <a:bodyPr/>
+      <a:lstStyle/>
+      <a:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </a:style>
+    </a:lnDef>
+  </a:objectDefaults>
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{2E142A2C-CD16-42D6-873A-C26D2A0506FA}" vid="{1BDDFF52-6CD6-40A5-AB3C-68EB2F1E4D0A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3559C712-7849-4583-85EC-520EB57A60E3}">
-  <dimension ref="A1:J1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF459F9E-703B-48EB-8666-D5D455A0584D}">
+  <dimension ref="A1:O1"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O11" sqref="O11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="9" width="10.25" customWidth="1"/>
-    <col min="10" max="10" width="11.5" customWidth="1"/>
+    <col min="1" max="9" width="10.875" customWidth="1"/>
+    <col min="10" max="12" width="12.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
         <v>9</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" t="s">
-        <v>8</v>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>

</xml_diff>

<commit_message>
feat: change behavior to easily detect and add students
</commit_message>
<xml_diff>
--- a/public/template/student.xlsx
+++ b/public/template/student.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\puntf\Desktop\CPE 402\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eltfshr/Desktop/inu-garden/public/template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CCFA536-0074-4FC1-BA34-D53460063F6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0428048B-B97A-A245-B523-D3A95CBDBAB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{E06D3729-24B1-455F-A1D9-8A924A109395}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="29040" windowHeight="15720" xr2:uid="{E06D3729-24B1-455F-A1D9-8A924A109395}"/>
   </bookViews>
   <sheets>
     <sheet name="Student" sheetId="1" r:id="rId1"/>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="679" uniqueCount="352">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="684" uniqueCount="357">
   <si>
     <t>_kmuttId</t>
   </si>
@@ -1108,6 +1108,21 @@
   </si>
   <si>
     <t>* ถ้าไม่มีข้อมูล ให้ใช้ ไม่ระบุ</t>
+  </si>
+  <si>
+    <t>* ชื่อไม่ต้องใส่คำนำหน้า</t>
+  </si>
+  <si>
+    <t>* ถ้าโรงเรียนไม่มีให้ใส่ ไม่ระบุ</t>
+  </si>
+  <si>
+    <t>* ข้อมูลอื่นที่ไม่มีให้ใส่ - ได้ยกเว้นเกรดต่างๆ ใส่เป็น 0 แทน</t>
+  </si>
+  <si>
+    <t>* สาขาและโรงเรียนมีให้เลือก แต่สามารถใส่ค่าอื่นได้</t>
+  </si>
+  <si>
+    <t>* ใส่ชื่อเป็น Eng หรือไทย ก็ได้ ชื่อกลางตัดออกได้ ระบบจะอ้างอิงทุกอย่างด้วยรหัสนักศึกษา</t>
   </si>
 </sst>
 </file>
@@ -1118,14 +1133,14 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Tahoma"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <charset val="222"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
-      <name val="Tahoma"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <charset val="222"/>
       <scheme val="minor"/>
@@ -1855,19 +1870,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF459F9E-703B-48EB-8666-D5D455A0584D}">
-  <dimension ref="A1:O1"/>
+  <dimension ref="A1:Q6"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="9" width="10.875" customWidth="1"/>
-    <col min="10" max="12" width="12.125" customWidth="1"/>
+    <col min="1" max="9" width="10.83203125" customWidth="1"/>
+    <col min="10" max="12" width="12.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1914,11 +1929,43 @@
         <v>14</v>
       </c>
     </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="Q2" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="Q3" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="Q4" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="Q5" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="Q6" t="s">
+        <v>355</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2:K5" xr:uid="{0A2EB8ED-AF76-49D2-848C-65E198DED9AB}">
+  <dataValidations count="3">
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="โรงเรียนไม่มีอยู่ในระบบ" error="ข้อความนี้เป็นการเพียงการเตือน สามารถใส่โรงเรียนที่ไม่มีข้อมูลได้ตามปกติ" sqref="K2:K5" xr:uid="{0A2EB8ED-AF76-49D2-848C-65E198DED9AB}">
       <formula1>INDIRECT("School[Used School]")</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:J5" xr:uid="{BDC42C86-9C31-C74C-8658-C4CEBA892D42}">
+      <formula1>0</formula1>
+      <formula2>4</formula2>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="ไม่มีข้อมูลสาขา" error="ข้อความนี้เป็นเพียงการเตือน สามารถใส่ข้อมูลสาขาที่ไม่มีในระบบได้" sqref="E2:E5" xr:uid="{A8114D8B-8997-434C-813F-B496F06C9D89}">
+      <formula1>"regular,international,rc,hds"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1932,14 +1979,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8505BE43-A73D-46D0-9236-7A548CA5D123}">
   <dimension ref="A1:E329"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="68.625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="75.125" customWidth="1"/>
+    <col min="1" max="1" width="68.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="75.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
feat: add student import example
</commit_message>
<xml_diff>
--- a/public/template/student.xlsx
+++ b/public/template/student.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eltfshr/Desktop/inu-garden/public/template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0428048B-B97A-A245-B523-D3A95CBDBAB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8B90D83-BA86-E248-9CEE-CF866A765EE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="29040" windowHeight="15720" xr2:uid="{E06D3729-24B1-455F-A1D9-8A924A109395}"/>
   </bookViews>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="684" uniqueCount="357">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="702" uniqueCount="365">
   <si>
     <t>_kmuttId</t>
   </si>
@@ -1123,6 +1123,30 @@
   </si>
   <si>
     <t>* ใส่ชื่อเป็น Eng หรือไทย ก็ได้ ชื่อกลางตัดออกได้ ระบบจะอ้างอิงทุกอย่างด้วยรหัสนักศึกษา</t>
+  </si>
+  <si>
+    <t>ชื่อ</t>
+  </si>
+  <si>
+    <t>นามกสุล</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>regular</t>
+  </si>
+  <si>
+    <t>computer engineer</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>lastname</t>
+  </si>
+  <si>
+    <t>international</t>
   </si>
 </sst>
 </file>
@@ -1930,11 +1954,101 @@
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>63070501000</v>
+      </c>
+      <c r="B2" t="s">
+        <v>357</v>
+      </c>
+      <c r="C2" t="s">
+        <v>358</v>
+      </c>
+      <c r="D2" t="s">
+        <v>359</v>
+      </c>
+      <c r="E2" t="s">
+        <v>360</v>
+      </c>
+      <c r="F2" t="s">
+        <v>361</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2" t="s">
+        <v>199</v>
+      </c>
+      <c r="L2" t="s">
+        <v>359</v>
+      </c>
+      <c r="M2">
+        <v>2566</v>
+      </c>
+      <c r="N2" t="s">
+        <v>359</v>
+      </c>
+      <c r="O2" t="s">
+        <v>359</v>
+      </c>
       <c r="Q2" t="s">
         <v>352</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>63070503400</v>
+      </c>
+      <c r="B3" t="s">
+        <v>362</v>
+      </c>
+      <c r="C3" t="s">
+        <v>363</v>
+      </c>
+      <c r="D3" t="s">
+        <v>359</v>
+      </c>
+      <c r="E3" t="s">
+        <v>364</v>
+      </c>
+      <c r="F3" t="s">
+        <v>361</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3" t="s">
+        <v>199</v>
+      </c>
+      <c r="L3" t="s">
+        <v>359</v>
+      </c>
+      <c r="M3">
+        <v>2566</v>
+      </c>
+      <c r="N3" t="s">
+        <v>359</v>
+      </c>
+      <c r="O3" t="s">
+        <v>359</v>
+      </c>
       <c r="Q3" t="s">
         <v>356</v>
       </c>

</xml_diff>